<commit_message>
[major] - added into the report the 2nd part by cdok
</commit_message>
<xml_diff>
--- a/bar_diagram.xlsx
+++ b/bar_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TheoO\github\adv_topics_in_DBs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9489283-A98D-4DAF-8D09-293DC61D3F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05DA0C3-F304-4C9C-801A-8E8117CF32BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="22710" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>RDD</t>
   </si>
@@ -49,6 +49,51 @@
   </si>
   <si>
     <t>Q5</t>
+  </si>
+  <si>
+    <t>10.34</t>
+  </si>
+  <si>
+    <t>19.95</t>
+  </si>
+  <si>
+    <t>16.74</t>
+  </si>
+  <si>
+    <t>63.6</t>
+  </si>
+  <si>
+    <t>63.1</t>
+  </si>
+  <si>
+    <t>75.44</t>
+  </si>
+  <si>
+    <t>72.3</t>
+  </si>
+  <si>
+    <t>18.8</t>
+  </si>
+  <si>
+    <t>69.53</t>
+  </si>
+  <si>
+    <t>17.89</t>
+  </si>
+  <si>
+    <t>14.26</t>
+  </si>
+  <si>
+    <t>86.92</t>
+  </si>
+  <si>
+    <t>161.39</t>
+  </si>
+  <si>
+    <t>9.27</t>
+  </si>
+  <si>
+    <t>289.01</t>
   </si>
 </sst>
 </file>
@@ -384,7 +429,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,25 +452,70 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[minor] - added distinct() in q3_rdd
</commit_message>
<xml_diff>
--- a/bar_diagram.xlsx
+++ b/bar_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TheoO\github\adv_topics_in_DBs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05DA0C3-F304-4C9C-801A-8E8117CF32BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C473E5A1-74F3-40E3-955E-964EB35DDAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>63.1</t>
   </si>
   <si>
-    <t>75.44</t>
-  </si>
-  <si>
     <t>72.3</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>289.01</t>
+  </si>
+  <si>
+    <t>73.75</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,13 +453,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -467,13 +467,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -481,7 +481,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -509,13 +509,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>